<commit_message>
added doc to xslxtojson
</commit_message>
<xml_diff>
--- a/ExcelSheets/Outside.xlsx
+++ b/ExcelSheets/Outside.xlsx
@@ -34,6 +34,93 @@
     <t>Folder</t>
   </si>
   <si>
+    <t>PHOTO_0019.jpg</t>
+  </si>
+  <si>
+    <t>47.65645277777778</t>
+  </si>
+  <si>
+    <t>-122.313675</t>
+  </si>
+  <si>
+    <t>2019:07:01 14:32:49</t>
+  </si>
+  <si>
+    <t>Outside</t>
+  </si>
+  <si>
+    <t>PHOTO_0033.jpg</t>
+  </si>
+  <si>
+    <t>47.65518333333333</t>
+  </si>
+  <si>
+    <t>-122.3097361111111</t>
+  </si>
+  <si>
+    <t>2019:07:01 16:42:14</t>
+  </si>
+  <si>
+    <t>PHOTO_0038.jpg</t>
+  </si>
+  <si>
+    <t>47.66025833333333</t>
+  </si>
+  <si>
+    <t>-122.30883333333333</t>
+  </si>
+  <si>
+    <t>2019:07:01 16:39:34</t>
+  </si>
+  <si>
+    <t>PHOTO_0361.jpg</t>
+  </si>
+  <si>
+    <t>47.648744444444446</t>
+  </si>
+  <si>
+    <t>-122.30970833333333</t>
+  </si>
+  <si>
+    <t>2019:07:11 12:23:44</t>
+  </si>
+  <si>
+    <t>PHOTO_0362.jpg</t>
+  </si>
+  <si>
+    <t>47.64862222222222</t>
+  </si>
+  <si>
+    <t>-122.30990833333333</t>
+  </si>
+  <si>
+    <t>2019:07:11 12:23:36</t>
+  </si>
+  <si>
+    <t>PHOTO_0363.jpg</t>
+  </si>
+  <si>
+    <t>47.64881666666667</t>
+  </si>
+  <si>
+    <t>-122.31033055555555</t>
+  </si>
+  <si>
+    <t>2019:07:11 12:23:28</t>
+  </si>
+  <si>
+    <t>PHOTO_0364.jpg</t>
+  </si>
+  <si>
+    <t>47.64888611111111</t>
+  </si>
+  <si>
+    <t>-122.31023888888889</t>
+  </si>
+  <si>
+    <t>2019:07:11 12:23:20</t>
+  </si>
+  <si>
     <t>PHOTO_0365.jpg</t>
   </si>
   <si>
@@ -46,7 +133,64 @@
     <t>2019:07:11 12:23:14</t>
   </si>
   <si>
-    <t>Outside</t>
+    <t>PHOTO_0366.jpg</t>
+  </si>
+  <si>
+    <t>47.64968611111111</t>
+  </si>
+  <si>
+    <t>-122.31140833333333</t>
+  </si>
+  <si>
+    <t>2019:07:11 12:23:07</t>
+  </si>
+  <si>
+    <t>PHOTO_0367.jpg</t>
+  </si>
+  <si>
+    <t>47.64979722222222</t>
+  </si>
+  <si>
+    <t>-122.31123333333333</t>
+  </si>
+  <si>
+    <t>2019:07:11 12:23:00</t>
+  </si>
+  <si>
+    <t>PHOTO_0368.jpg</t>
+  </si>
+  <si>
+    <t>47.649858333333334</t>
+  </si>
+  <si>
+    <t>-122.31134444444444</t>
+  </si>
+  <si>
+    <t>2019:07:11 12:22:53</t>
+  </si>
+  <si>
+    <t>PHOTO_0369.jpg</t>
+  </si>
+  <si>
+    <t>47.64971944444444</t>
+  </si>
+  <si>
+    <t>-122.31145</t>
+  </si>
+  <si>
+    <t>2019:07:11 12:22:46</t>
+  </si>
+  <si>
+    <t>PHOTO_0370.jpg</t>
+  </si>
+  <si>
+    <t>47.649877777777775</t>
+  </si>
+  <si>
+    <t>-122.31213055555556</t>
+  </si>
+  <si>
+    <t>2019:07:11 12:22:39</t>
   </si>
   <si>
     <t>PHOTO_0371.jpg</t>
@@ -61,42 +205,6 @@
     <t>2019:07:11 12:22:32</t>
   </si>
   <si>
-    <t>PHOTO_0370.jpg</t>
-  </si>
-  <si>
-    <t>47.649877777777775</t>
-  </si>
-  <si>
-    <t>-122.31213055555556</t>
-  </si>
-  <si>
-    <t>2019:07:11 12:22:39</t>
-  </si>
-  <si>
-    <t>PHOTO_0364.jpg</t>
-  </si>
-  <si>
-    <t>47.64888611111111</t>
-  </si>
-  <si>
-    <t>-122.31023888888889</t>
-  </si>
-  <si>
-    <t>2019:07:11 12:23:20</t>
-  </si>
-  <si>
-    <t>PHOTO_0038.jpg</t>
-  </si>
-  <si>
-    <t>47.66025833333333</t>
-  </si>
-  <si>
-    <t>-122.30883333333333</t>
-  </si>
-  <si>
-    <t>2019:07:01 16:39:34</t>
-  </si>
-  <si>
     <t>PHOTO_0372.jpg</t>
   </si>
   <si>
@@ -109,30 +217,6 @@
     <t>2019:07:11 12:22:24</t>
   </si>
   <si>
-    <t>PHOTO_0366.jpg</t>
-  </si>
-  <si>
-    <t>47.64968611111111</t>
-  </si>
-  <si>
-    <t>-122.31140833333333</t>
-  </si>
-  <si>
-    <t>2019:07:11 12:23:07</t>
-  </si>
-  <si>
-    <t>PHOTO_0367.jpg</t>
-  </si>
-  <si>
-    <t>47.64979722222222</t>
-  </si>
-  <si>
-    <t>-122.31123333333333</t>
-  </si>
-  <si>
-    <t>2019:07:11 12:23:00</t>
-  </si>
-  <si>
     <t>PHOTO_0373.jpg</t>
   </si>
   <si>
@@ -145,30 +229,6 @@
     <t>2019:07:11 12:22:16</t>
   </si>
   <si>
-    <t>PHOTO_0363.jpg</t>
-  </si>
-  <si>
-    <t>47.64881666666667</t>
-  </si>
-  <si>
-    <t>-122.31033055555555</t>
-  </si>
-  <si>
-    <t>2019:07:11 12:23:28</t>
-  </si>
-  <si>
-    <t>PHOTO_0362.jpg</t>
-  </si>
-  <si>
-    <t>47.64862222222222</t>
-  </si>
-  <si>
-    <t>-122.30990833333333</t>
-  </si>
-  <si>
-    <t>2019:07:11 12:23:36</t>
-  </si>
-  <si>
     <t>PHOTO_0374.jpg</t>
   </si>
   <si>
@@ -191,66 +251,6 @@
   </si>
   <si>
     <t>2019:07:11 12:21:59</t>
-  </si>
-  <si>
-    <t>PHOTO_0361.jpg</t>
-  </si>
-  <si>
-    <t>47.648744444444446</t>
-  </si>
-  <si>
-    <t>-122.30970833333333</t>
-  </si>
-  <si>
-    <t>2019:07:11 12:23:44</t>
-  </si>
-  <si>
-    <t>PHOTO_0033.jpg</t>
-  </si>
-  <si>
-    <t>47.65518333333333</t>
-  </si>
-  <si>
-    <t>-122.3097361111111</t>
-  </si>
-  <si>
-    <t>2019:07:01 16:42:14</t>
-  </si>
-  <si>
-    <t>PHOTO_0019.jpg</t>
-  </si>
-  <si>
-    <t>47.65645277777778</t>
-  </si>
-  <si>
-    <t>-122.313675</t>
-  </si>
-  <si>
-    <t>2019:07:01 14:32:49</t>
-  </si>
-  <si>
-    <t>PHOTO_0369.jpg</t>
-  </si>
-  <si>
-    <t>47.64971944444444</t>
-  </si>
-  <si>
-    <t>-122.31145</t>
-  </si>
-  <si>
-    <t>2019:07:11 12:22:46</t>
-  </si>
-  <si>
-    <t>PHOTO_0368.jpg</t>
-  </si>
-  <si>
-    <t>47.649858333333334</t>
-  </si>
-  <si>
-    <t>-122.31134444444444</t>
-  </si>
-  <si>
-    <t>2019:07:11 12:22:53</t>
   </si>
 </sst>
 </file>

</xml_diff>